<commit_message>
Fixed infinite loop edge case
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camde\Documents\UiPath\Spate Monthly Trend Report\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C045432-861F-4478-8FDD-EC106CEE96F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E43625-99BC-4539-935B-FD8EB55743AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15890" yWindow="5070" windowWidth="17620" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lists" sheetId="1" r:id="rId1"/>
@@ -721,18 +721,18 @@
       <selection sqref="A1:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.54296875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
-    <col min="10" max="25" width="8.7109375" customWidth="1"/>
+    <col min="10" max="25" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="14.25" customHeight="1">
@@ -799,7 +799,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" ht="14.5">
       <c r="A3" s="2" t="s">
         <v>40</v>
       </c>
@@ -845,7 +845,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" ht="14.5">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -1917,15 +1917,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBD2794A-1B96-4FD6-A77D-1D625F5D34D4}">
   <dimension ref="A1:Z1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" customWidth="1"/>
-    <col min="3" max="3" width="98.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.7265625" customWidth="1"/>
+    <col min="2" max="2" width="29.7265625" customWidth="1"/>
+    <col min="3" max="3" width="98.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1971,16 +1971,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2017,23 +2017,23 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
         <v>26</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>34</v>
@@ -2142,7 +2142,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="45">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -3136,12 +3136,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.81640625" customWidth="1"/>
+    <col min="2" max="2" width="30.1796875" customWidth="1"/>
+    <col min="3" max="3" width="60.26953125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>